<commit_message>
Add costs for compressors and storage
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_SUP_H2NewTechs.xlsx
+++ b/SubRES_TMPL/SubRES_SUP_H2NewTechs.xlsx
@@ -1,25 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TIMES-models\TIM\SubRES_TMPL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TIMES-models\TIM\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75442F6F-32A4-469F-8644-9E39DF048451}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{177DF63C-133C-47C8-9AD6-E38623CBEA11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43080" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8010" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tech_data" sheetId="1" r:id="rId1"/>
     <sheet name="processes" sheetId="2" r:id="rId2"/>
     <sheet name="commodities" sheetId="3" r:id="rId3"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId4"/>
-  </externalReferences>
   <definedNames>
     <definedName name="__123Graph_AEUMILKPN" hidden="1">#REF!</definedName>
     <definedName name="_AtRisk_SimSetting_AutomaticallyGenerateReports" hidden="1">FALSE</definedName>
@@ -342,7 +339,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -388,15 +385,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -412,30 +408,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
-      <sheetName val="SUP_H2Storage"/>
-      <sheetName val="Cover"/>
-      <sheetName val="SUP_H2Production"/>
-      <sheetName val="SUP_H2Liquefaction"/>
-      <sheetName val="SUP_H2Delivery"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -703,8 +675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:O24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I32" sqref="I31:I32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -952,7 +924,7 @@
         <f>487*1.35</f>
         <v>657.45</v>
       </c>
-      <c r="N11" s="6">
+      <c r="N11" s="3">
         <f t="shared" ref="N11:N15" si="1">M11*0.014</f>
         <v>9.2043000000000017</v>
       </c>
@@ -972,7 +944,7 @@
         <f>360*1.35</f>
         <v>486.00000000000006</v>
       </c>
-      <c r="N12" s="6">
+      <c r="N12" s="3">
         <f t="shared" si="1"/>
         <v>6.8040000000000012</v>
       </c>
@@ -985,7 +957,7 @@
         <f>268*1.35</f>
         <v>361.8</v>
       </c>
-      <c r="N13" s="6">
+      <c r="N13" s="3">
         <f t="shared" si="1"/>
         <v>5.0651999999999999</v>
       </c>
@@ -998,7 +970,7 @@
         <f>202*1.35</f>
         <v>272.70000000000005</v>
       </c>
-      <c r="N14" s="6">
+      <c r="N14" s="3">
         <f t="shared" si="1"/>
         <v>3.8178000000000005</v>
       </c>
@@ -1018,7 +990,7 @@
         <f>138*1.35</f>
         <v>186.3</v>
       </c>
-      <c r="N15" s="6">
+      <c r="N15" s="3">
         <f t="shared" si="1"/>
         <v>2.6082000000000001</v>
       </c>
@@ -1053,7 +1025,7 @@
       <c r="N16" s="2"/>
       <c r="O16" s="2"/>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B17" t="str">
         <f>processes!C7</f>
         <v>SH2COMPM_01</v>
@@ -1068,14 +1040,21 @@
       <c r="E17" t="s">
         <v>64</v>
       </c>
-      <c r="G17" s="7">
+      <c r="G17">
         <v>2023</v>
       </c>
       <c r="H17">
         <v>2023</v>
       </c>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="M17">
+        <v>7.06</v>
+      </c>
+      <c r="N17" s="6">
+        <f>M17*0.02</f>
+        <v>0.14119999999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B18" t="str">
         <f>processes!C8</f>
         <v>SH2COMPH_01</v>
@@ -1090,14 +1069,21 @@
       <c r="E18" t="s">
         <v>52</v>
       </c>
-      <c r="G18" s="7">
+      <c r="G18">
         <v>2023</v>
       </c>
       <c r="H18">
         <v>2023</v>
       </c>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="M18">
+        <v>9.48</v>
+      </c>
+      <c r="N18" s="6">
+        <f>M18*0.02</f>
+        <v>0.18960000000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B19" t="str">
         <f>processes!C9</f>
         <v>SH2LSTG_01</v>
@@ -1112,8 +1098,14 @@
       <c r="E19" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="G19">
+        <v>2023</v>
+      </c>
+      <c r="H19">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B20" t="str">
         <f>processes!C10</f>
         <v>SH2GMPSTG_01</v>
@@ -1128,8 +1120,21 @@
       <c r="E20" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="G20">
+        <v>2023</v>
+      </c>
+      <c r="H20">
+        <v>2023</v>
+      </c>
+      <c r="M20">
+        <v>6.9999999999999999E-4</v>
+      </c>
+      <c r="N20">
+        <f>M20*0.02</f>
+        <v>1.4E-5</v>
+      </c>
+    </row>
+    <row r="21" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B21" t="str">
         <f>processes!C11</f>
         <v>SH2GHPSTG_01</v>
@@ -1144,8 +1149,14 @@
       <c r="E21" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="G21">
+        <v>2023</v>
+      </c>
+      <c r="H21">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="22" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B22" t="str">
         <f>processes!C12</f>
         <v>SH2LDEL_01</v>
@@ -1160,8 +1171,14 @@
       <c r="E22" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="G22">
+        <v>2023</v>
+      </c>
+      <c r="H22">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="23" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B23" t="str">
         <f>processes!C13</f>
         <v>SH2GMDEL_01</v>
@@ -1176,8 +1193,14 @@
       <c r="E23" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="G23">
+        <v>2023</v>
+      </c>
+      <c r="H23">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="24" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B24" t="str">
         <f>processes!C14</f>
         <v>SH2GHDEL_01</v>
@@ -1191,6 +1214,12 @@
       </c>
       <c r="E24" t="s">
         <v>53</v>
+      </c>
+      <c r="G24">
+        <v>2023</v>
+      </c>
+      <c r="H24">
+        <v>2023</v>
       </c>
     </row>
   </sheetData>
@@ -1202,8 +1231,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A60D4C0D-EE5B-4CEE-B57E-E0841322AD53}">
   <dimension ref="B2:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
Add temp efficiency values for compression and transport
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_SUP_H2NewTechs.xlsx
+++ b/SubRES_TMPL/SubRES_SUP_H2NewTechs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TIMES-models\TIM\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{177DF63C-133C-47C8-9AD6-E38623CBEA11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E971EA5-FDDE-4D6C-88E9-EB263047DF40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8010" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="43080" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tech_data" sheetId="1" r:id="rId1"/>
@@ -104,7 +104,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="76">
   <si>
     <t>~FI_Process</t>
   </si>
@@ -385,7 +385,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -393,6 +393,7 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -676,7 +677,7 @@
   <dimension ref="B2:O24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1010,14 +1011,18 @@
       <c r="E16" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="F16" s="2"/>
+      <c r="F16" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="G16" s="2">
         <v>2023</v>
       </c>
       <c r="H16" s="2">
         <v>2023</v>
       </c>
-      <c r="I16" s="2"/>
+      <c r="I16" s="2">
+        <v>1</v>
+      </c>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
@@ -1040,11 +1045,17 @@
       <c r="E17" t="s">
         <v>64</v>
       </c>
+      <c r="F17" s="7" t="s">
+        <v>74</v>
+      </c>
       <c r="G17">
         <v>2023</v>
       </c>
       <c r="H17">
         <v>2023</v>
+      </c>
+      <c r="I17">
+        <v>1</v>
       </c>
       <c r="M17">
         <v>7.06</v>
@@ -1069,11 +1080,17 @@
       <c r="E18" t="s">
         <v>52</v>
       </c>
+      <c r="F18" s="7" t="s">
+        <v>74</v>
+      </c>
       <c r="G18">
         <v>2023</v>
       </c>
       <c r="H18">
         <v>2023</v>
+      </c>
+      <c r="I18">
+        <v>1</v>
       </c>
       <c r="M18">
         <v>9.48</v>
@@ -1171,11 +1188,17 @@
       <c r="E22" t="s">
         <v>51</v>
       </c>
+      <c r="F22" t="s">
+        <v>74</v>
+      </c>
       <c r="G22">
         <v>2023</v>
       </c>
       <c r="H22">
         <v>2023</v>
+      </c>
+      <c r="I22">
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.45">
@@ -1193,11 +1216,17 @@
       <c r="E23" t="s">
         <v>54</v>
       </c>
+      <c r="F23" t="s">
+        <v>74</v>
+      </c>
       <c r="G23">
         <v>2023</v>
       </c>
       <c r="H23">
         <v>2023</v>
+      </c>
+      <c r="I23">
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.45">
@@ -1215,11 +1244,17 @@
       <c r="E24" t="s">
         <v>53</v>
       </c>
+      <c r="F24" t="s">
+        <v>74</v>
+      </c>
       <c r="G24">
         <v>2023</v>
       </c>
       <c r="H24">
         <v>2023</v>
+      </c>
+      <c r="I24">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Redefine efficiency of electrolysis
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_SUP_H2NewTechs.xlsx
+++ b/SubRES_TMPL/SubRES_SUP_H2NewTechs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TIMES-models\TIM\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E971EA5-FDDE-4D6C-88E9-EB263047DF40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF56B5D7-E541-4E4E-AC23-E9E4608A59ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="43080" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -338,9 +338,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.000"/>
-  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -385,15 +382,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -677,7 +673,7 @@
   <dimension ref="B2:O24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -769,8 +765,9 @@
       <c r="H4">
         <v>2023</v>
       </c>
-      <c r="I4">
-        <v>0.66500000000000004</v>
+      <c r="I4" s="5">
+        <f>1/0.665</f>
+        <v>1.5037593984962405</v>
       </c>
       <c r="J4">
         <v>25</v>
@@ -795,6 +792,7 @@
       <c r="G5">
         <v>2025</v>
       </c>
+      <c r="I5" s="5"/>
       <c r="M5" s="3">
         <f>688*1.6</f>
         <v>1100.8</v>
@@ -813,7 +811,7 @@
       </c>
       <c r="I6" s="5">
         <f>I4*1.04</f>
-        <v>0.6916000000000001</v>
+        <v>1.5639097744360901</v>
       </c>
       <c r="M6" s="3">
         <f>509*1.6</f>
@@ -828,6 +826,7 @@
       <c r="G7">
         <v>2035</v>
       </c>
+      <c r="I7" s="5"/>
       <c r="M7" s="3">
         <f>380*1.6</f>
         <v>608</v>
@@ -841,6 +840,7 @@
       <c r="G8">
         <v>2040</v>
       </c>
+      <c r="I8" s="5"/>
       <c r="M8" s="3">
         <f>285*1.6</f>
         <v>456</v>
@@ -859,7 +859,7 @@
       </c>
       <c r="I9" s="5">
         <f>I6*1.14</f>
-        <v>0.78842400000000001</v>
+        <v>1.7828571428571427</v>
       </c>
       <c r="M9" s="3">
         <f>195*1.6</f>
@@ -894,8 +894,9 @@
       <c r="H10" s="2">
         <v>2023</v>
       </c>
-      <c r="I10" s="2">
-        <v>0.66500000000000004</v>
+      <c r="I10" s="6">
+        <f>1/0.665</f>
+        <v>1.5037593984962405</v>
       </c>
       <c r="J10" s="2">
         <v>25</v>
@@ -921,6 +922,7 @@
       <c r="G11">
         <v>2025</v>
       </c>
+      <c r="I11" s="5"/>
       <c r="M11" s="3">
         <f>487*1.35</f>
         <v>657.45</v>
@@ -939,7 +941,7 @@
       </c>
       <c r="I12" s="5">
         <f>I10*1.04</f>
-        <v>0.6916000000000001</v>
+        <v>1.5639097744360901</v>
       </c>
       <c r="M12" s="3">
         <f>360*1.35</f>
@@ -954,6 +956,7 @@
       <c r="G13">
         <v>2035</v>
       </c>
+      <c r="I13" s="5"/>
       <c r="M13" s="3">
         <f>268*1.35</f>
         <v>361.8</v>
@@ -967,6 +970,7 @@
       <c r="G14">
         <v>2040</v>
       </c>
+      <c r="I14" s="5"/>
       <c r="M14" s="3">
         <f>202*1.35</f>
         <v>272.70000000000005</v>
@@ -985,7 +989,7 @@
       </c>
       <c r="I15" s="5">
         <f>I12*1.14</f>
-        <v>0.78842400000000001</v>
+        <v>1.7828571428571427</v>
       </c>
       <c r="M15" s="3">
         <f>138*1.35</f>
@@ -1045,7 +1049,7 @@
       <c r="E17" t="s">
         <v>64</v>
       </c>
-      <c r="F17" s="7" t="s">
+      <c r="F17" t="s">
         <v>74</v>
       </c>
       <c r="G17">
@@ -1060,7 +1064,7 @@
       <c r="M17">
         <v>7.06</v>
       </c>
-      <c r="N17" s="6">
+      <c r="N17" s="5">
         <f>M17*0.02</f>
         <v>0.14119999999999999</v>
       </c>
@@ -1080,7 +1084,7 @@
       <c r="E18" t="s">
         <v>52</v>
       </c>
-      <c r="F18" s="7" t="s">
+      <c r="F18" t="s">
         <v>74</v>
       </c>
       <c r="G18">
@@ -1095,7 +1099,7 @@
       <c r="M18">
         <v>9.48</v>
       </c>
-      <c r="N18" s="6">
+      <c r="N18" s="5">
         <f>M18*0.02</f>
         <v>0.18960000000000002</v>
       </c>

</xml_diff>

<commit_message>
Adjust transport and compression
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_SUP_H2NewTechs.xlsx
+++ b/SubRES_TMPL/SubRES_SUP_H2NewTechs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TIMES-models\TIM\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF56B5D7-E541-4E4E-AC23-E9E4608A59ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E6CA08D-05CD-42FE-83E4-10AD4850CC93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43080" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tech_data" sheetId="1" r:id="rId1"/>
@@ -103,8 +103,26 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={CDD9769C-BE5C-42BD-B1CC-5A12FA7F4A7D}</author>
+  </authors>
+  <commentList>
+    <comment ref="N23" authorId="0" shapeId="0" xr:uid="{CDD9769C-BE5C-42BD-B1CC-5A12FA7F4A7D}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Multiply by distance in km</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="77">
   <si>
     <t>~FI_Process</t>
   </si>
@@ -332,19 +350,35 @@
   </si>
   <si>
     <t>NCAP_AFA</t>
+  </si>
+  <si>
+    <t>STG_EFF</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -382,7 +416,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -390,6 +424,9 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -405,6 +442,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Olexandr Balyk" id="{E9E8DD3A-8C00-45EF-943C-98E543523E42}" userId="78cf518dc4778786" providerId="Windows Live"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -668,36 +711,46 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="N23" dT="2023-12-18T05:21:17.87" personId="{E9E8DD3A-8C00-45EF-943C-98E543523E42}" id="{CDD9769C-BE5C-42BD-B1CC-5A12FA7F4A7D}">
+    <text>Multiply by distance in km</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:O24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B2:P24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+      <selection activeCell="N29" sqref="N29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="46.19921875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.33203125" customWidth="1"/>
-    <col min="6" max="6" width="13.265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.33203125" customWidth="1"/>
-    <col min="8" max="9" width="11.53125" customWidth="1"/>
-    <col min="10" max="10" width="10.59765625" customWidth="1"/>
-    <col min="11" max="11" width="11.53125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.796875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.73046875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="11.5703125" customWidth="1"/>
+    <col min="11" max="11" width="10.5703125" customWidth="1"/>
+    <col min="12" max="12" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:16" x14ac:dyDescent="0.25">
       <c r="G2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
@@ -723,25 +776,28 @@
         <v>72</v>
       </c>
       <c r="J3" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="O3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="P3" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B4" t="str">
         <f>processes!C4</f>
         <v>SH2PELC_01S</v>
@@ -769,40 +825,42 @@
         <f>1/0.665</f>
         <v>1.5037593984962405</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="5"/>
+      <c r="K4">
         <v>25</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <f>8760*3.6/1000</f>
         <v>31.536000000000001</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <v>0.97</v>
       </c>
-      <c r="M4" s="3">
+      <c r="N4" s="5">
         <f>791*1.6</f>
         <v>1265.6000000000001</v>
       </c>
-      <c r="N4" s="3">
-        <f>M4*0.041</f>
+      <c r="O4" s="3">
+        <f>N4*0.041</f>
         <v>51.889600000000009</v>
       </c>
     </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="G5">
         <v>2025</v>
       </c>
       <c r="I5" s="5"/>
-      <c r="M5" s="3">
+      <c r="J5" s="5"/>
+      <c r="N5" s="5">
         <f>688*1.6</f>
         <v>1100.8</v>
       </c>
-      <c r="N5" s="3">
-        <f t="shared" ref="N5:N9" si="0">M5*0.041</f>
+      <c r="O5" s="3">
+        <f t="shared" ref="O5:O9" si="0">N5*0.041</f>
         <v>45.132800000000003</v>
       </c>
     </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
       <c r="F6" t="s">
         <v>74</v>
       </c>
@@ -813,44 +871,47 @@
         <f>I4*1.04</f>
         <v>1.5639097744360901</v>
       </c>
-      <c r="M6" s="3">
+      <c r="J6" s="5"/>
+      <c r="N6" s="5">
         <f>509*1.6</f>
         <v>814.40000000000009</v>
       </c>
-      <c r="N6" s="3">
+      <c r="O6" s="3">
         <f t="shared" si="0"/>
         <v>33.390400000000007</v>
       </c>
     </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
       <c r="G7">
         <v>2035</v>
       </c>
       <c r="I7" s="5"/>
-      <c r="M7" s="3">
+      <c r="J7" s="5"/>
+      <c r="N7" s="5">
         <f>380*1.6</f>
         <v>608</v>
       </c>
-      <c r="N7" s="3">
+      <c r="O7" s="3">
         <f t="shared" si="0"/>
         <v>24.928000000000001</v>
       </c>
     </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
       <c r="G8">
         <v>2040</v>
       </c>
       <c r="I8" s="5"/>
-      <c r="M8" s="3">
+      <c r="J8" s="5"/>
+      <c r="N8" s="5">
         <f>285*1.6</f>
         <v>456</v>
       </c>
-      <c r="N8" s="3">
+      <c r="O8" s="3">
         <f t="shared" si="0"/>
         <v>18.696000000000002</v>
       </c>
     </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
       <c r="F9" t="s">
         <v>74</v>
       </c>
@@ -861,16 +922,17 @@
         <f>I6*1.14</f>
         <v>1.7828571428571427</v>
       </c>
-      <c r="M9" s="3">
+      <c r="J9" s="5"/>
+      <c r="N9" s="5">
         <f>195*1.6</f>
         <v>312</v>
       </c>
-      <c r="N9" s="3">
+      <c r="O9" s="3">
         <f t="shared" si="0"/>
         <v>12.792</v>
       </c>
     </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="str">
         <f>processes!C5</f>
         <v>SH2PELC_01L</v>
@@ -898,41 +960,43 @@
         <f>1/0.665</f>
         <v>1.5037593984962405</v>
       </c>
-      <c r="J10" s="2">
+      <c r="J10" s="6"/>
+      <c r="K10" s="2">
         <v>25</v>
       </c>
-      <c r="K10" s="2">
+      <c r="L10" s="2">
         <f>8760*3.6/1000</f>
         <v>31.536000000000001</v>
       </c>
-      <c r="L10" s="2">
+      <c r="M10" s="2">
         <v>0.97</v>
       </c>
-      <c r="M10" s="4">
+      <c r="N10" s="6">
         <f>560*1.35</f>
         <v>756</v>
       </c>
-      <c r="N10" s="4">
-        <f>M10*0.014</f>
+      <c r="O10" s="4">
+        <f>N10*0.014</f>
         <v>10.584</v>
       </c>
-      <c r="O10" s="2"/>
-    </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="P10" s="2"/>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
       <c r="G11">
         <v>2025</v>
       </c>
       <c r="I11" s="5"/>
-      <c r="M11" s="3">
+      <c r="J11" s="5"/>
+      <c r="N11" s="5">
         <f>487*1.35</f>
         <v>657.45</v>
       </c>
-      <c r="N11" s="3">
-        <f t="shared" ref="N11:N15" si="1">M11*0.014</f>
+      <c r="O11" s="3">
+        <f t="shared" ref="O11:O15" si="1">N11*0.014</f>
         <v>9.2043000000000017</v>
       </c>
     </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
       <c r="F12" t="s">
         <v>74</v>
       </c>
@@ -943,44 +1007,47 @@
         <f>I10*1.04</f>
         <v>1.5639097744360901</v>
       </c>
-      <c r="M12" s="3">
+      <c r="J12" s="5"/>
+      <c r="N12" s="5">
         <f>360*1.35</f>
         <v>486.00000000000006</v>
       </c>
-      <c r="N12" s="3">
+      <c r="O12" s="3">
         <f t="shared" si="1"/>
         <v>6.8040000000000012</v>
       </c>
     </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
       <c r="G13">
         <v>2035</v>
       </c>
       <c r="I13" s="5"/>
-      <c r="M13" s="3">
+      <c r="J13" s="5"/>
+      <c r="N13" s="5">
         <f>268*1.35</f>
         <v>361.8</v>
       </c>
-      <c r="N13" s="3">
+      <c r="O13" s="3">
         <f t="shared" si="1"/>
         <v>5.0651999999999999</v>
       </c>
     </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
       <c r="G14">
         <v>2040</v>
       </c>
       <c r="I14" s="5"/>
-      <c r="M14" s="3">
+      <c r="J14" s="5"/>
+      <c r="N14" s="5">
         <f>202*1.35</f>
         <v>272.70000000000005</v>
       </c>
-      <c r="N14" s="3">
+      <c r="O14" s="3">
         <f t="shared" si="1"/>
         <v>3.8178000000000005</v>
       </c>
     </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
       <c r="F15" t="s">
         <v>74</v>
       </c>
@@ -991,16 +1058,17 @@
         <f>I12*1.14</f>
         <v>1.7828571428571427</v>
       </c>
-      <c r="M15" s="3">
+      <c r="J15" s="5"/>
+      <c r="N15" s="5">
         <f>138*1.35</f>
         <v>186.3</v>
       </c>
-      <c r="N15" s="3">
+      <c r="O15" s="3">
         <f t="shared" si="1"/>
         <v>2.6082000000000001</v>
       </c>
     </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="str">
         <f>processes!C6</f>
         <v>SH2LIQ_01</v>
@@ -1028,13 +1096,23 @@
         <v>1</v>
       </c>
       <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
+      <c r="K16" s="7">
+        <v>30</v>
+      </c>
+      <c r="L16" s="2">
+        <v>1</v>
+      </c>
       <c r="M16" s="2"/>
-      <c r="N16" s="2"/>
-      <c r="O16" s="2"/>
-    </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.45">
+      <c r="N16" s="6">
+        <v>6.56</v>
+      </c>
+      <c r="O16" s="6">
+        <f>N16*0.04</f>
+        <v>0.26239999999999997</v>
+      </c>
+      <c r="P16" s="2"/>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B17" t="str">
         <f>processes!C7</f>
         <v>SH2COMPM_01</v>
@@ -1061,15 +1139,21 @@
       <c r="I17">
         <v>1</v>
       </c>
-      <c r="M17">
+      <c r="K17" s="8">
+        <v>30</v>
+      </c>
+      <c r="L17">
+        <v>1</v>
+      </c>
+      <c r="N17" s="5">
         <v>7.06</v>
       </c>
-      <c r="N17" s="5">
-        <f>M17*0.02</f>
+      <c r="O17" s="5">
+        <f>N17*0.02</f>
         <v>0.14119999999999999</v>
       </c>
     </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B18" t="str">
         <f>processes!C8</f>
         <v>SH2COMPH_01</v>
@@ -1096,15 +1180,21 @@
       <c r="I18">
         <v>1</v>
       </c>
-      <c r="M18">
+      <c r="K18" s="8">
+        <v>30</v>
+      </c>
+      <c r="L18">
+        <v>1</v>
+      </c>
+      <c r="N18" s="5">
         <v>9.48</v>
       </c>
-      <c r="N18" s="5">
-        <f>M18*0.02</f>
+      <c r="O18" s="5">
+        <f>N18*0.02</f>
         <v>0.18960000000000002</v>
       </c>
     </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B19" t="str">
         <f>processes!C9</f>
         <v>SH2LSTG_01</v>
@@ -1125,8 +1215,24 @@
       <c r="H19">
         <v>2023</v>
       </c>
-    </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.45">
+      <c r="J19" s="8">
+        <v>1</v>
+      </c>
+      <c r="K19">
+        <v>30</v>
+      </c>
+      <c r="L19">
+        <v>1</v>
+      </c>
+      <c r="N19" s="5">
+        <v>250</v>
+      </c>
+      <c r="O19">
+        <f>N19*0.02</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B20" t="str">
         <f>processes!C10</f>
         <v>SH2GMPSTG_01</v>
@@ -1147,15 +1253,24 @@
       <c r="H20">
         <v>2023</v>
       </c>
-      <c r="M20">
-        <v>6.9999999999999999E-4</v>
-      </c>
-      <c r="N20">
-        <f>M20*0.02</f>
-        <v>1.4E-5</v>
-      </c>
-    </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.45">
+      <c r="J20" s="8">
+        <v>1</v>
+      </c>
+      <c r="K20" s="8">
+        <v>30</v>
+      </c>
+      <c r="L20">
+        <v>1</v>
+      </c>
+      <c r="N20" s="5">
+        <v>185.49</v>
+      </c>
+      <c r="O20" s="5">
+        <f>N20*0.02</f>
+        <v>3.7098000000000004</v>
+      </c>
+    </row>
+    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B21" t="str">
         <f>processes!C11</f>
         <v>SH2GHPSTG_01</v>
@@ -1176,8 +1291,24 @@
       <c r="H21">
         <v>2023</v>
       </c>
-    </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.45">
+      <c r="J21" s="8">
+        <v>1</v>
+      </c>
+      <c r="K21" s="8">
+        <v>30</v>
+      </c>
+      <c r="L21">
+        <v>1</v>
+      </c>
+      <c r="N21" s="5">
+        <v>5000</v>
+      </c>
+      <c r="O21">
+        <f>N21*0.02</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B22" t="str">
         <f>processes!C12</f>
         <v>SH2LDEL_01</v>
@@ -1201,11 +1332,24 @@
       <c r="H22">
         <v>2023</v>
       </c>
-      <c r="I22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.45">
+      <c r="I22" s="8">
+        <v>1</v>
+      </c>
+      <c r="K22" s="8">
+        <v>15</v>
+      </c>
+      <c r="L22">
+        <v>1</v>
+      </c>
+      <c r="N22" s="9">
+        <v>1</v>
+      </c>
+      <c r="O22" s="5">
+        <f>N22*0.02</f>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B23" t="str">
         <f>processes!C13</f>
         <v>SH2GMDEL_01</v>
@@ -1229,11 +1373,24 @@
       <c r="H23">
         <v>2023</v>
       </c>
-      <c r="I23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.45">
+      <c r="I23" s="8">
+        <v>1</v>
+      </c>
+      <c r="K23" s="8">
+        <v>50</v>
+      </c>
+      <c r="L23">
+        <v>1</v>
+      </c>
+      <c r="N23" s="9">
+        <v>1</v>
+      </c>
+      <c r="O23">
+        <f>N23*0.02</f>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B24" t="str">
         <f>processes!C14</f>
         <v>SH2GHDEL_01</v>
@@ -1257,12 +1414,26 @@
       <c r="H24">
         <v>2023</v>
       </c>
-      <c r="I24">
-        <v>1</v>
+      <c r="I24" s="8">
+        <v>1</v>
+      </c>
+      <c r="K24" s="8">
+        <v>15</v>
+      </c>
+      <c r="L24">
+        <v>1</v>
+      </c>
+      <c r="N24" s="9">
+        <v>1</v>
+      </c>
+      <c r="O24">
+        <f>N24*0.02</f>
+        <v>0.02</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1271,23 +1442,23 @@
   <dimension ref="B2:I14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="15.46484375" customWidth="1"/>
-    <col min="4" max="4" width="52.73046875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.53125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" customWidth="1"/>
+    <col min="4" max="4" width="52.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1313,7 +1484,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>9</v>
       </c>
@@ -1339,7 +1510,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>9</v>
       </c>
@@ -1365,7 +1536,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>9</v>
       </c>
@@ -1385,7 +1556,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>9</v>
       </c>
@@ -1405,7 +1576,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>9</v>
       </c>
@@ -1425,7 +1596,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>18</v>
       </c>
@@ -1445,7 +1616,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>18</v>
       </c>
@@ -1465,7 +1636,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>18</v>
       </c>
@@ -1485,7 +1656,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>9</v>
       </c>
@@ -1505,7 +1676,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>9</v>
       </c>
@@ -1525,7 +1696,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>9</v>
       </c>
@@ -1558,19 +1729,19 @@
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="11.1328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.59765625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>42</v>
       </c>
@@ -1596,7 +1767,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>50</v>
       </c>
@@ -1610,7 +1781,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>53</v>
       </c>
@@ -1621,7 +1792,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>54</v>
       </c>

</xml_diff>

<commit_message>
Add a hydrogen export process
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_SUP_H2NewTechs.xlsx
+++ b/SubRES_TMPL/SubRES_SUP_H2NewTechs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TIMES-models\TIM\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E6CA08D-05CD-42FE-83E4-10AD4850CC93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B43068E8-471F-4A58-A555-747676DFD869}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -122,7 +122,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="83">
   <si>
     <t>~FI_Process</t>
   </si>
@@ -353,13 +353,31 @@
   </si>
   <si>
     <t>STG_EFF</t>
+  </si>
+  <si>
+    <t>IRE</t>
+  </si>
+  <si>
+    <t>EXPH2GMD</t>
+  </si>
+  <si>
+    <t>Hydrogen (medium pressure gas) - export</t>
+  </si>
+  <si>
+    <t>annual</t>
+  </si>
+  <si>
+    <t>exp</t>
+  </si>
+  <si>
+    <t>IRE_PRICE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -373,12 +391,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -721,10 +733,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:P24"/>
+  <dimension ref="B2:Q25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N29" sqref="N29"/>
+      <selection activeCell="P25" sqref="P25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -745,12 +757,12 @@
     <col min="17" max="17" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:17" x14ac:dyDescent="0.25">
       <c r="G2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
@@ -796,8 +808,11 @@
       <c r="P3" s="1" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q3" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B4" t="str">
         <f>processes!C4</f>
         <v>SH2PELC_01S</v>
@@ -845,7 +860,7 @@
         <v>51.889600000000009</v>
       </c>
     </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
       <c r="G5">
         <v>2025</v>
       </c>
@@ -860,7 +875,7 @@
         <v>45.132800000000003</v>
       </c>
     </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
       <c r="F6" t="s">
         <v>74</v>
       </c>
@@ -881,7 +896,7 @@
         <v>33.390400000000007</v>
       </c>
     </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
       <c r="G7">
         <v>2035</v>
       </c>
@@ -896,7 +911,7 @@
         <v>24.928000000000001</v>
       </c>
     </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
       <c r="G8">
         <v>2040</v>
       </c>
@@ -911,7 +926,7 @@
         <v>18.696000000000002</v>
       </c>
     </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
       <c r="F9" t="s">
         <v>74</v>
       </c>
@@ -932,7 +947,7 @@
         <v>12.792</v>
       </c>
     </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="str">
         <f>processes!C5</f>
         <v>SH2PELC_01L</v>
@@ -981,7 +996,7 @@
       </c>
       <c r="P10" s="2"/>
     </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
       <c r="G11">
         <v>2025</v>
       </c>
@@ -996,7 +1011,7 @@
         <v>9.2043000000000017</v>
       </c>
     </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
       <c r="F12" t="s">
         <v>74</v>
       </c>
@@ -1017,7 +1032,7 @@
         <v>6.8040000000000012</v>
       </c>
     </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
       <c r="G13">
         <v>2035</v>
       </c>
@@ -1032,7 +1047,7 @@
         <v>5.0651999999999999</v>
       </c>
     </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
       <c r="G14">
         <v>2040</v>
       </c>
@@ -1047,7 +1062,7 @@
         <v>3.8178000000000005</v>
       </c>
     </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
       <c r="F15" t="s">
         <v>74</v>
       </c>
@@ -1068,7 +1083,7 @@
         <v>2.6082000000000001</v>
       </c>
     </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="str">
         <f>processes!C6</f>
         <v>SH2LIQ_01</v>
@@ -1112,7 +1127,7 @@
       </c>
       <c r="P16" s="2"/>
     </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B17" t="str">
         <f>processes!C7</f>
         <v>SH2COMPM_01</v>
@@ -1149,11 +1164,11 @@
         <v>7.06</v>
       </c>
       <c r="O17" s="5">
-        <f>N17*0.02</f>
+        <f t="shared" ref="O17:O24" si="2">N17*0.02</f>
         <v>0.14119999999999999</v>
       </c>
     </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B18" t="str">
         <f>processes!C8</f>
         <v>SH2COMPH_01</v>
@@ -1190,11 +1205,11 @@
         <v>9.48</v>
       </c>
       <c r="O18" s="5">
-        <f>N18*0.02</f>
+        <f t="shared" si="2"/>
         <v>0.18960000000000002</v>
       </c>
     </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B19" t="str">
         <f>processes!C9</f>
         <v>SH2LSTG_01</v>
@@ -1228,11 +1243,11 @@
         <v>250</v>
       </c>
       <c r="O19">
-        <f>N19*0.02</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B20" t="str">
         <f>processes!C10</f>
         <v>SH2GMPSTG_01</v>
@@ -1266,11 +1281,11 @@
         <v>185.49</v>
       </c>
       <c r="O20" s="5">
-        <f>N20*0.02</f>
+        <f t="shared" si="2"/>
         <v>3.7098000000000004</v>
       </c>
     </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B21" t="str">
         <f>processes!C11</f>
         <v>SH2GHPSTG_01</v>
@@ -1304,11 +1319,11 @@
         <v>5000</v>
       </c>
       <c r="O21">
-        <f>N21*0.02</f>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
     </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B22" t="str">
         <f>processes!C12</f>
         <v>SH2LDEL_01</v>
@@ -1345,11 +1360,11 @@
         <v>1</v>
       </c>
       <c r="O22" s="5">
-        <f>N22*0.02</f>
+        <f t="shared" si="2"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B23" t="str">
         <f>processes!C13</f>
         <v>SH2GMDEL_01</v>
@@ -1386,11 +1401,11 @@
         <v>1</v>
       </c>
       <c r="O23">
-        <f>N23*0.02</f>
+        <f t="shared" si="2"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B24" t="str">
         <f>processes!C14</f>
         <v>SH2GHDEL_01</v>
@@ -1427,8 +1442,34 @@
         <v>1</v>
       </c>
       <c r="O24">
-        <f>N24*0.02</f>
+        <f t="shared" si="2"/>
         <v>0.02</v>
+      </c>
+    </row>
+    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B25" t="str">
+        <f>processes!C15</f>
+        <v>EXPH2GMD</v>
+      </c>
+      <c r="C25" t="str">
+        <f>processes!D15</f>
+        <v>Hydrogen (medium pressure gas) - export</v>
+      </c>
+      <c r="D25" t="s">
+        <v>54</v>
+      </c>
+      <c r="F25" t="s">
+        <v>81</v>
+      </c>
+      <c r="G25">
+        <v>2023</v>
+      </c>
+      <c r="H25">
+        <v>2023</v>
+      </c>
+      <c r="Q25">
+        <f>5*0.12</f>
+        <v>0.6</v>
       </c>
     </row>
   </sheetData>
@@ -1439,10 +1480,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A60D4C0D-EE5B-4CEE-B57E-E0841322AD53}">
-  <dimension ref="B2:I14"/>
+  <dimension ref="B2:I15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1714,6 +1755,26 @@
       </c>
       <c r="G14" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>77</v>
+      </c>
+      <c r="C15" t="s">
+        <v>78</v>
+      </c>
+      <c r="D15" t="s">
+        <v>79</v>
+      </c>
+      <c r="E15" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Redefine Hydrogen commodities on DayNite level
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_SUP_H2NewTechs.xlsx
+++ b/SubRES_TMPL/SubRES_SUP_H2NewTechs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TIMES-models\TIM\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B43068E8-471F-4A58-A555-747676DFD869}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DFA62E7-15A7-4C36-8E08-076A0AC52E43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tech_data" sheetId="1" r:id="rId1"/>
@@ -122,7 +122,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="84">
   <si>
     <t>~FI_Process</t>
   </si>
@@ -371,6 +371,9 @@
   </si>
   <si>
     <t>IRE_PRICE</t>
+  </si>
+  <si>
+    <t>DayNite</t>
   </si>
 </sst>
 </file>
@@ -735,8 +738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:Q25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P25" sqref="P25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1786,8 +1789,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33ED947B-68CF-4216-9D00-DDF150F9577F}">
   <dimension ref="B2:I6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1841,6 +1844,9 @@
       <c r="E4" t="s">
         <v>10</v>
       </c>
+      <c r="G4" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
@@ -1852,6 +1858,9 @@
       <c r="E5" t="s">
         <v>10</v>
       </c>
+      <c r="G5" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
@@ -1862,6 +1871,9 @@
       </c>
       <c r="E6" t="s">
         <v>10</v>
+      </c>
+      <c r="G6" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Include SUPELC consumption in compression and liquefaction
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_SUP_H2NewTechs.xlsx
+++ b/SubRES_TMPL/SubRES_SUP_H2NewTechs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TIMES-models\TIM\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DFA62E7-15A7-4C36-8E08-076A0AC52E43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9277F5A3-00F6-462B-88AF-0022689E3CE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-75" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tech_data" sheetId="1" r:id="rId1"/>
@@ -109,7 +109,7 @@
     <author>tc={CDD9769C-BE5C-42BD-B1CC-5A12FA7F4A7D}</author>
   </authors>
   <commentList>
-    <comment ref="N23" authorId="0" shapeId="0" xr:uid="{CDD9769C-BE5C-42BD-B1CC-5A12FA7F4A7D}">
+    <comment ref="P26" authorId="0" shapeId="0" xr:uid="{CDD9769C-BE5C-42BD-B1CC-5A12FA7F4A7D}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -122,7 +122,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="87">
   <si>
     <t>~FI_Process</t>
   </si>
@@ -355,9 +355,6 @@
     <t>STG_EFF</t>
   </si>
   <si>
-    <t>IRE</t>
-  </si>
-  <si>
     <t>EXPH2GMD</t>
   </si>
   <si>
@@ -374,12 +371,27 @@
   </si>
   <si>
     <t>DayNite</t>
+  </si>
+  <si>
+    <t>EXP</t>
+  </si>
+  <si>
+    <t>Comm-IN-A</t>
+  </si>
+  <si>
+    <t>FLO_EFF</t>
+  </si>
+  <si>
+    <t>SUPELC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -431,7 +443,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -442,6 +454,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -728,7 +745,7 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="N23" dT="2023-12-18T05:21:17.87" personId="{E9E8DD3A-8C00-45EF-943C-98E543523E42}" id="{CDD9769C-BE5C-42BD-B1CC-5A12FA7F4A7D}">
+  <threadedComment ref="P26" dT="2023-12-18T05:21:17.87" personId="{E9E8DD3A-8C00-45EF-943C-98E543523E42}" id="{CDD9769C-BE5C-42BD-B1CC-5A12FA7F4A7D}">
     <text>Multiply by distance in km</text>
   </threadedComment>
 </ThreadedComments>
@@ -736,36 +753,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:Q25"/>
+  <dimension ref="B2:S28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="49.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="11.5703125" customWidth="1"/>
-    <col min="11" max="11" width="10.5703125" customWidth="1"/>
-    <col min="12" max="12" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="11.5703125" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="G2" t="s">
+    <row r="2" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="H2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
@@ -776,46 +794,52 @@
         <v>27</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="L3" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="O3" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="P3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="Q3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="R3" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="Q3" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="S3" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B4" t="str">
         <f>processes!C4</f>
         <v>SH2PELC_01S</v>
@@ -827,130 +851,136 @@
       <c r="D4" t="s">
         <v>60</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>61</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>74</v>
       </c>
-      <c r="G4">
-        <v>2023</v>
-      </c>
       <c r="H4">
         <v>2023</v>
       </c>
-      <c r="I4" s="5">
+      <c r="I4">
+        <v>2023</v>
+      </c>
+      <c r="J4" s="5">
         <f>1/0.665</f>
         <v>1.5037593984962405</v>
       </c>
-      <c r="J4" s="5"/>
-      <c r="K4">
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4">
         <v>25</v>
       </c>
-      <c r="L4">
+      <c r="N4">
         <f>8760*3.6/1000</f>
         <v>31.536000000000001</v>
       </c>
-      <c r="M4">
+      <c r="O4">
         <v>0.97</v>
       </c>
-      <c r="N4" s="5">
+      <c r="P4" s="5">
         <f>791*1.6</f>
         <v>1265.6000000000001</v>
       </c>
-      <c r="O4" s="3">
-        <f>N4*0.041</f>
+      <c r="Q4" s="3">
+        <f>P4*0.041</f>
         <v>51.889600000000009</v>
       </c>
     </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="G5">
+    <row r="5" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="H5">
         <v>2025</v>
       </c>
-      <c r="I5" s="5"/>
       <c r="J5" s="5"/>
-      <c r="N5" s="5">
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="P5" s="5">
         <f>688*1.6</f>
         <v>1100.8</v>
       </c>
-      <c r="O5" s="3">
-        <f t="shared" ref="O5:O9" si="0">N5*0.041</f>
+      <c r="Q5" s="3">
+        <f t="shared" ref="Q5:Q9" si="0">P5*0.041</f>
         <v>45.132800000000003</v>
       </c>
     </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="F6" t="s">
+    <row r="6" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
         <v>74</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>2030</v>
       </c>
-      <c r="I6" s="5">
-        <f>I4*1.04</f>
+      <c r="J6" s="5">
+        <f>J4*1.04</f>
         <v>1.5639097744360901</v>
       </c>
-      <c r="J6" s="5"/>
-      <c r="N6" s="5">
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="P6" s="5">
         <f>509*1.6</f>
         <v>814.40000000000009</v>
       </c>
-      <c r="O6" s="3">
+      <c r="Q6" s="3">
         <f t="shared" si="0"/>
         <v>33.390400000000007</v>
       </c>
     </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="G7">
+    <row r="7" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="H7">
         <v>2035</v>
       </c>
-      <c r="I7" s="5"/>
       <c r="J7" s="5"/>
-      <c r="N7" s="5">
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="P7" s="5">
         <f>380*1.6</f>
         <v>608</v>
       </c>
-      <c r="O7" s="3">
+      <c r="Q7" s="3">
         <f t="shared" si="0"/>
         <v>24.928000000000001</v>
       </c>
     </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="G8">
+    <row r="8" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="H8">
         <v>2040</v>
       </c>
-      <c r="I8" s="5"/>
       <c r="J8" s="5"/>
-      <c r="N8" s="5">
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="P8" s="5">
         <f>285*1.6</f>
         <v>456</v>
       </c>
-      <c r="O8" s="3">
+      <c r="Q8" s="3">
         <f t="shared" si="0"/>
         <v>18.696000000000002</v>
       </c>
     </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="F9" t="s">
+    <row r="9" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="G9" t="s">
         <v>74</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>2050</v>
       </c>
-      <c r="I9" s="5">
-        <f>I6*1.14</f>
+      <c r="J9" s="5">
+        <f>J6*1.14</f>
         <v>1.7828571428571427</v>
       </c>
-      <c r="J9" s="5"/>
-      <c r="N9" s="5">
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="P9" s="5">
         <f>195*1.6</f>
         <v>312</v>
       </c>
-      <c r="O9" s="3">
+      <c r="Q9" s="3">
         <f t="shared" si="0"/>
         <v>12.792</v>
       </c>
     </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="str">
         <f>processes!C5</f>
         <v>SH2PELC_01L</v>
@@ -962,131 +992,138 @@
       <c r="D10" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="2"/>
+      <c r="F10" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="G10" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="G10" s="2">
-        <v>2023</v>
-      </c>
       <c r="H10" s="2">
         <v>2023</v>
       </c>
-      <c r="I10" s="6">
+      <c r="I10" s="2">
+        <v>2023</v>
+      </c>
+      <c r="J10" s="6">
         <f>1/0.665</f>
         <v>1.5037593984962405</v>
       </c>
-      <c r="J10" s="6"/>
-      <c r="K10" s="2">
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="2">
         <v>25</v>
       </c>
-      <c r="L10" s="2">
+      <c r="N10" s="2">
         <f>8760*3.6/1000</f>
         <v>31.536000000000001</v>
       </c>
-      <c r="M10" s="2">
+      <c r="O10" s="2">
         <v>0.97</v>
       </c>
-      <c r="N10" s="6">
+      <c r="P10" s="6">
         <f>560*1.35</f>
         <v>756</v>
       </c>
-      <c r="O10" s="4">
-        <f>N10*0.014</f>
+      <c r="Q10" s="4">
+        <f>P10*0.014</f>
         <v>10.584</v>
       </c>
-      <c r="P10" s="2"/>
-    </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="G11">
+      <c r="R10" s="2"/>
+    </row>
+    <row r="11" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="H11">
         <v>2025</v>
       </c>
-      <c r="I11" s="5"/>
       <c r="J11" s="5"/>
-      <c r="N11" s="5">
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="P11" s="5">
         <f>487*1.35</f>
         <v>657.45</v>
       </c>
-      <c r="O11" s="3">
-        <f t="shared" ref="O11:O15" si="1">N11*0.014</f>
+      <c r="Q11" s="3">
+        <f t="shared" ref="Q11:Q15" si="1">P11*0.014</f>
         <v>9.2043000000000017</v>
       </c>
     </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="F12" t="s">
+    <row r="12" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="G12" t="s">
         <v>74</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>2030</v>
       </c>
-      <c r="I12" s="5">
-        <f>I10*1.04</f>
+      <c r="J12" s="5">
+        <f>J10*1.04</f>
         <v>1.5639097744360901</v>
       </c>
-      <c r="J12" s="5"/>
-      <c r="N12" s="5">
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="P12" s="5">
         <f>360*1.35</f>
         <v>486.00000000000006</v>
       </c>
-      <c r="O12" s="3">
+      <c r="Q12" s="3">
         <f t="shared" si="1"/>
         <v>6.8040000000000012</v>
       </c>
     </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="G13">
+    <row r="13" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="H13">
         <v>2035</v>
       </c>
-      <c r="I13" s="5"/>
       <c r="J13" s="5"/>
-      <c r="N13" s="5">
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="P13" s="5">
         <f>268*1.35</f>
         <v>361.8</v>
       </c>
-      <c r="O13" s="3">
+      <c r="Q13" s="3">
         <f t="shared" si="1"/>
         <v>5.0651999999999999</v>
       </c>
     </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="G14">
+    <row r="14" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="H14">
         <v>2040</v>
       </c>
-      <c r="I14" s="5"/>
       <c r="J14" s="5"/>
-      <c r="N14" s="5">
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
+      <c r="P14" s="5">
         <f>202*1.35</f>
         <v>272.70000000000005</v>
       </c>
-      <c r="O14" s="3">
+      <c r="Q14" s="3">
         <f t="shared" si="1"/>
         <v>3.8178000000000005</v>
       </c>
     </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="F15" t="s">
+    <row r="15" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="G15" t="s">
         <v>74</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <v>2050</v>
       </c>
-      <c r="I15" s="5">
-        <f>I12*1.14</f>
+      <c r="J15" s="5">
+        <f>J12*1.14</f>
         <v>1.7828571428571427</v>
       </c>
-      <c r="J15" s="5"/>
-      <c r="N15" s="5">
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
+      <c r="P15" s="5">
         <f>138*1.35</f>
         <v>186.3</v>
       </c>
-      <c r="O15" s="3">
+      <c r="Q15" s="3">
         <f t="shared" si="1"/>
         <v>2.6082000000000001</v>
       </c>
     </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="str">
         <f>processes!C6</f>
         <v>SH2LIQ_01</v>
@@ -1098,379 +1135,448 @@
       <c r="D16" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E16" s="2"/>
+      <c r="F16" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="G16" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="G16" s="2">
-        <v>2023</v>
-      </c>
       <c r="H16" s="2">
         <v>2023</v>
       </c>
       <c r="I16" s="2">
-        <v>1</v>
-      </c>
-      <c r="J16" s="2"/>
-      <c r="K16" s="7">
+        <v>2023</v>
+      </c>
+      <c r="J16" s="2">
+        <v>1</v>
+      </c>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="7">
         <v>30</v>
       </c>
-      <c r="L16" s="2">
-        <v>1</v>
-      </c>
-      <c r="M16" s="2"/>
-      <c r="N16" s="6">
+      <c r="N16" s="2">
+        <v>1</v>
+      </c>
+      <c r="O16" s="2"/>
+      <c r="P16" s="6">
         <v>6.56</v>
       </c>
-      <c r="O16" s="6">
-        <f>N16*0.04</f>
+      <c r="Q16" s="6">
+        <f>P16*0.04</f>
         <v>0.26239999999999997</v>
       </c>
-      <c r="P16" s="2"/>
-    </row>
-    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B17" t="str">
+      <c r="R16" s="2"/>
+    </row>
+    <row r="17" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="F17" s="10"/>
+      <c r="G17" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="H17" s="13">
+        <v>2023</v>
+      </c>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="14">
+        <f>10.25*3.6/120</f>
+        <v>0.3075</v>
+      </c>
+      <c r="L17" s="10"/>
+      <c r="M17" s="11"/>
+      <c r="N17" s="10"/>
+      <c r="O17" s="10"/>
+      <c r="P17" s="12"/>
+      <c r="Q17" s="12"/>
+      <c r="R17" s="10"/>
+    </row>
+    <row r="18" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B18" t="str">
         <f>processes!C7</f>
         <v>SH2COMPM_01</v>
       </c>
-      <c r="C17" t="str">
+      <c r="C18" t="str">
         <f>processes!D7</f>
         <v>Compression medium (100 bar)</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D18" t="s">
         <v>61</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F18" t="s">
         <v>64</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G18" t="s">
         <v>74</v>
       </c>
-      <c r="G17">
-        <v>2023</v>
-      </c>
-      <c r="H17">
-        <v>2023</v>
-      </c>
-      <c r="I17">
-        <v>1</v>
-      </c>
-      <c r="K17" s="8">
+      <c r="H18">
+        <v>2023</v>
+      </c>
+      <c r="I18">
+        <v>2023</v>
+      </c>
+      <c r="J18">
+        <v>1</v>
+      </c>
+      <c r="M18" s="8">
         <v>30</v>
       </c>
-      <c r="L17">
-        <v>1</v>
-      </c>
-      <c r="N17" s="5">
+      <c r="N18">
+        <v>1</v>
+      </c>
+      <c r="P18" s="5">
         <v>7.06</v>
       </c>
-      <c r="O17" s="5">
-        <f t="shared" ref="O17:O24" si="2">N17*0.02</f>
+      <c r="Q18" s="5">
+        <f t="shared" ref="Q18:Q27" si="2">P18*0.02</f>
         <v>0.14119999999999999</v>
       </c>
     </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B18" t="str">
+    <row r="19" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
+        <v>86</v>
+      </c>
+      <c r="G19" t="s">
+        <v>74</v>
+      </c>
+      <c r="H19">
+        <v>2023</v>
+      </c>
+      <c r="K19" s="14">
+        <f>0.9*3.6/120</f>
+        <v>2.7000000000000003E-2</v>
+      </c>
+      <c r="M19" s="8"/>
+      <c r="P19" s="5"/>
+      <c r="Q19" s="5"/>
+    </row>
+    <row r="20" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B20" t="str">
         <f>processes!C8</f>
         <v>SH2COMPH_01</v>
       </c>
-      <c r="C18" t="str">
+      <c r="C20" t="str">
         <f>processes!D8</f>
         <v>Compression high (500 bar)</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D20" t="s">
         <v>61</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F20" t="s">
         <v>52</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G20" t="s">
         <v>74</v>
       </c>
-      <c r="G18">
-        <v>2023</v>
-      </c>
-      <c r="H18">
-        <v>2023</v>
-      </c>
-      <c r="I18">
-        <v>1</v>
-      </c>
-      <c r="K18" s="8">
+      <c r="H20">
+        <v>2023</v>
+      </c>
+      <c r="I20">
+        <v>2023</v>
+      </c>
+      <c r="J20">
+        <v>1</v>
+      </c>
+      <c r="M20" s="8">
         <v>30</v>
       </c>
-      <c r="L18">
-        <v>1</v>
-      </c>
-      <c r="N18" s="5">
+      <c r="N20">
+        <v>1</v>
+      </c>
+      <c r="P20" s="5">
         <v>9.48</v>
       </c>
-      <c r="O18" s="5">
+      <c r="Q20" s="5">
         <f t="shared" si="2"/>
         <v>0.18960000000000002</v>
       </c>
     </row>
-    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B19" t="str">
+    <row r="21" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="E21" t="s">
+        <v>86</v>
+      </c>
+      <c r="G21" t="s">
+        <v>74</v>
+      </c>
+      <c r="H21">
+        <v>2023</v>
+      </c>
+      <c r="K21" s="14">
+        <f>2.6*3.6/120</f>
+        <v>7.8000000000000014E-2</v>
+      </c>
+      <c r="M21" s="8"/>
+      <c r="P21" s="5"/>
+      <c r="Q21" s="5"/>
+    </row>
+    <row r="22" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B22" t="str">
         <f>processes!C9</f>
         <v>SH2LSTG_01</v>
       </c>
-      <c r="C19" t="str">
+      <c r="C22" t="str">
         <f>processes!D9</f>
         <v>Hydrogen storage - liquid</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D22" t="s">
         <v>63</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F22" t="s">
         <v>63</v>
       </c>
-      <c r="G19">
-        <v>2023</v>
-      </c>
-      <c r="H19">
-        <v>2023</v>
-      </c>
-      <c r="J19" s="8">
-        <v>1</v>
-      </c>
-      <c r="K19">
+      <c r="H22">
+        <v>2023</v>
+      </c>
+      <c r="I22">
+        <v>2023</v>
+      </c>
+      <c r="L22" s="8">
+        <v>1</v>
+      </c>
+      <c r="M22">
         <v>30</v>
       </c>
-      <c r="L19">
-        <v>1</v>
-      </c>
-      <c r="N19" s="5">
+      <c r="N22">
+        <v>1</v>
+      </c>
+      <c r="P22" s="5">
         <v>250</v>
       </c>
-      <c r="O19">
+      <c r="Q22">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B20" t="str">
+    <row r="23" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B23" t="str">
         <f>processes!C10</f>
         <v>SH2GMPSTG_01</v>
       </c>
-      <c r="C20" t="str">
+      <c r="C23" t="str">
         <f>processes!D10</f>
         <v>Hydrogen storage - gas medium pressure (salt cavern)</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D23" t="s">
         <v>64</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F23" t="s">
         <v>64</v>
       </c>
-      <c r="G20">
-        <v>2023</v>
-      </c>
-      <c r="H20">
-        <v>2023</v>
-      </c>
-      <c r="J20" s="8">
-        <v>1</v>
-      </c>
-      <c r="K20" s="8">
+      <c r="H23">
+        <v>2023</v>
+      </c>
+      <c r="I23">
+        <v>2023</v>
+      </c>
+      <c r="L23" s="8">
+        <v>1</v>
+      </c>
+      <c r="M23" s="8">
         <v>30</v>
       </c>
-      <c r="L20">
-        <v>1</v>
-      </c>
-      <c r="N20" s="5">
+      <c r="N23">
+        <v>1</v>
+      </c>
+      <c r="P23" s="5">
         <v>185.49</v>
       </c>
-      <c r="O20" s="5">
+      <c r="Q23" s="5">
         <f t="shared" si="2"/>
         <v>3.7098000000000004</v>
       </c>
     </row>
-    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B21" t="str">
+    <row r="24" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B24" t="str">
         <f>processes!C11</f>
         <v>SH2GHPSTG_01</v>
       </c>
-      <c r="C21" t="str">
+      <c r="C24" t="str">
         <f>processes!D11</f>
         <v>Hydrogen storage - gas high pressure (tanks)</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D24" t="s">
         <v>52</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F24" t="s">
         <v>52</v>
       </c>
-      <c r="G21">
-        <v>2023</v>
-      </c>
-      <c r="H21">
-        <v>2023</v>
-      </c>
-      <c r="J21" s="8">
-        <v>1</v>
-      </c>
-      <c r="K21" s="8">
+      <c r="H24">
+        <v>2023</v>
+      </c>
+      <c r="I24">
+        <v>2023</v>
+      </c>
+      <c r="L24" s="8">
+        <v>1</v>
+      </c>
+      <c r="M24" s="8">
         <v>30</v>
       </c>
-      <c r="L21">
-        <v>1</v>
-      </c>
-      <c r="N21" s="5">
+      <c r="N24">
+        <v>1</v>
+      </c>
+      <c r="P24" s="5">
         <v>5000</v>
       </c>
-      <c r="O21">
+      <c r="Q24">
         <f t="shared" si="2"/>
         <v>100</v>
       </c>
     </row>
-    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B22" t="str">
+    <row r="25" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B25" t="str">
         <f>processes!C12</f>
         <v>SH2LDEL_01</v>
       </c>
-      <c r="C22" t="str">
+      <c r="C25" t="str">
         <f>processes!D12</f>
         <v>Hydrogen (liquid) delivery - road tanker</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D25" t="s">
         <v>63</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F25" t="s">
         <v>51</v>
       </c>
-      <c r="F22" t="s">
+      <c r="G25" t="s">
         <v>74</v>
       </c>
-      <c r="G22">
-        <v>2023</v>
-      </c>
-      <c r="H22">
-        <v>2023</v>
-      </c>
-      <c r="I22" s="8">
-        <v>1</v>
-      </c>
-      <c r="K22" s="8">
+      <c r="H25">
+        <v>2023</v>
+      </c>
+      <c r="I25">
+        <v>2023</v>
+      </c>
+      <c r="J25" s="8">
+        <v>1</v>
+      </c>
+      <c r="K25" s="8"/>
+      <c r="M25" s="8">
         <v>15</v>
       </c>
-      <c r="L22">
-        <v>1</v>
-      </c>
-      <c r="N22" s="9">
-        <v>1</v>
-      </c>
-      <c r="O22" s="5">
+      <c r="N25">
+        <v>1</v>
+      </c>
+      <c r="P25" s="9">
+        <v>1</v>
+      </c>
+      <c r="Q25" s="5">
         <f t="shared" si="2"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B23" t="str">
+    <row r="26" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B26" t="str">
         <f>processes!C13</f>
         <v>SH2GMDEL_01</v>
       </c>
-      <c r="C23" t="str">
+      <c r="C26" t="str">
         <f>processes!D13</f>
         <v>Hydrogen (medium pressure gas) delivery - pipeline</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D26" t="s">
         <v>64</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F26" t="s">
         <v>54</v>
       </c>
-      <c r="F23" t="s">
+      <c r="G26" t="s">
         <v>74</v>
       </c>
-      <c r="G23">
-        <v>2023</v>
-      </c>
-      <c r="H23">
-        <v>2023</v>
-      </c>
-      <c r="I23" s="8">
-        <v>1</v>
-      </c>
-      <c r="K23" s="8">
+      <c r="H26">
+        <v>2023</v>
+      </c>
+      <c r="I26">
+        <v>2023</v>
+      </c>
+      <c r="J26" s="8">
+        <v>1</v>
+      </c>
+      <c r="K26" s="8"/>
+      <c r="M26" s="8">
         <v>50</v>
       </c>
-      <c r="L23">
-        <v>1</v>
-      </c>
-      <c r="N23" s="9">
-        <v>1</v>
-      </c>
-      <c r="O23">
+      <c r="N26">
+        <v>1</v>
+      </c>
+      <c r="P26" s="9">
+        <v>1</v>
+      </c>
+      <c r="Q26">
         <f t="shared" si="2"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B24" t="str">
+    <row r="27" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B27" t="str">
         <f>processes!C14</f>
         <v>SH2GHDEL_01</v>
       </c>
-      <c r="C24" t="str">
+      <c r="C27" t="str">
         <f>processes!D14</f>
         <v>Hydrogen (high pressure gas) delivery - tube trailer</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D27" t="s">
         <v>52</v>
       </c>
-      <c r="E24" t="s">
+      <c r="F27" t="s">
         <v>53</v>
       </c>
-      <c r="F24" t="s">
+      <c r="G27" t="s">
         <v>74</v>
       </c>
-      <c r="G24">
-        <v>2023</v>
-      </c>
-      <c r="H24">
-        <v>2023</v>
-      </c>
-      <c r="I24" s="8">
-        <v>1</v>
-      </c>
-      <c r="K24" s="8">
+      <c r="H27">
+        <v>2023</v>
+      </c>
+      <c r="I27">
+        <v>2023</v>
+      </c>
+      <c r="J27" s="8">
+        <v>1</v>
+      </c>
+      <c r="K27" s="8"/>
+      <c r="M27" s="8">
         <v>15</v>
       </c>
-      <c r="L24">
-        <v>1</v>
-      </c>
-      <c r="N24" s="9">
-        <v>1</v>
-      </c>
-      <c r="O24">
+      <c r="N27">
+        <v>1</v>
+      </c>
+      <c r="P27" s="9">
+        <v>1</v>
+      </c>
+      <c r="Q27">
         <f t="shared" si="2"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B25" t="str">
+    <row r="28" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B28" t="str">
         <f>processes!C15</f>
         <v>EXPH2GMD</v>
       </c>
-      <c r="C25" t="str">
+      <c r="C28" t="str">
         <f>processes!D15</f>
         <v>Hydrogen (medium pressure gas) - export</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D28" t="s">
         <v>54</v>
       </c>
-      <c r="F25" t="s">
-        <v>81</v>
-      </c>
-      <c r="G25">
-        <v>2023</v>
-      </c>
-      <c r="H25">
-        <v>2023</v>
-      </c>
-      <c r="Q25">
+      <c r="G28" t="s">
+        <v>80</v>
+      </c>
+      <c r="H28">
+        <v>2023</v>
+      </c>
+      <c r="I28">
+        <v>2023</v>
+      </c>
+      <c r="S28">
         <f>5*0.12</f>
         <v>0.6</v>
       </c>
@@ -1486,14 +1592,14 @@
   <dimension ref="B2:I15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="15.42578125" customWidth="1"/>
     <col min="4" max="4" width="52.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1762,13 +1868,13 @@
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
+        <v>83</v>
+      </c>
+      <c r="C15" t="s">
         <v>77</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>78</v>
-      </c>
-      <c r="D15" t="s">
-        <v>79</v>
       </c>
       <c r="E15" t="s">
         <v>10</v>
@@ -1777,7 +1883,7 @@
         <v>11</v>
       </c>
       <c r="G15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1789,8 +1895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33ED947B-68CF-4216-9D00-DDF150F9577F}">
   <dimension ref="B2:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1845,7 +1951,7 @@
         <v>10</v>
       </c>
       <c r="G4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
@@ -1859,7 +1965,7 @@
         <v>10</v>
       </c>
       <c r="G5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
@@ -1873,7 +1979,7 @@
         <v>10</v>
       </c>
       <c r="G6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>